<commit_message>
change xlsx to csv
</commit_message>
<xml_diff>
--- a/server/test/csv_parser/files/molecules.xlsx
+++ b/server/test/csv_parser/files/molecules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\ParserTests\CSVFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\csv_parser\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7DA6AF-435D-4B3C-A892-018AE87062C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4808EEF-E2AF-4CE5-84FD-0514928A13BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$T$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$S$142</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -33,7 +33,7 @@
     <author>alclairet (B12819)</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1371,28 +1371,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U171"/>
+  <dimension ref="A1:T171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="18.33203125" style="4" customWidth="1"/>
     <col min="4" max="5" width="33.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="34.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" style="2" customWidth="1"/>
-    <col min="11" max="21" width="20.33203125" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="11.44140625" style="2"/>
+    <col min="6" max="6" width="34.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="2" customWidth="1"/>
+    <col min="10" max="20" width="20.33203125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1408,14 +1408,17 @@
       <c r="E1" s="4" t="s">
         <v>226</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="G1" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>231</v>
@@ -1427,7 +1430,7 @@
         <v>231</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>232</v>
@@ -1436,7 +1439,7 @@
         <v>232</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>233</v>
@@ -1445,16 +1448,13 @@
         <v>233</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="U1" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1470,20 +1470,20 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="J2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1499,17 +1499,17 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U3" s="2">
+      <c r="T3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1525,14 +1525,14 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1546,26 +1546,26 @@
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2" t="s">
         <v>239</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="U5" s="2">
+      <c r="T5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1579,17 +1579,17 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="J6" s="21"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1603,14 +1603,14 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -1622,14 +1622,14 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1641,14 +1641,14 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -1660,20 +1660,20 @@
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -1685,17 +1685,17 @@
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F11" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -1707,14 +1707,14 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
@@ -1726,14 +1726,14 @@
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
@@ -1745,14 +1745,14 @@
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
@@ -1764,14 +1764,14 @@
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
@@ -1783,14 +1783,14 @@
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>31</v>
       </c>
@@ -1802,14 +1802,14 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>32</v>
       </c>
@@ -1821,14 +1821,14 @@
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
@@ -1840,20 +1840,20 @@
       <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="I19" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
@@ -1865,20 +1865,20 @@
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="I20" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -1890,17 +1890,17 @@
       <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
@@ -1912,17 +1912,17 @@
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>41</v>
       </c>
@@ -1934,26 +1934,26 @@
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="I23" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="J23" s="2" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>48</v>
       </c>
@@ -1965,15 +1965,15 @@
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="J24" s="2" t="s">
+      <c r="G24" s="15"/>
+      <c r="I24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>46</v>
       </c>
@@ -1985,15 +1985,15 @@
       <c r="E25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="J25" s="2" t="s">
+      <c r="G25" s="15"/>
+      <c r="I25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>49</v>
       </c>
@@ -2005,15 +2005,15 @@
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="J26" s="2" t="s">
+      <c r="G26" s="15"/>
+      <c r="I26" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>50</v>
       </c>
@@ -2025,15 +2025,15 @@
       <c r="E27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="J27" s="2" t="s">
+      <c r="G27" s="15"/>
+      <c r="I27" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>47</v>
       </c>
@@ -2045,15 +2045,15 @@
       <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="J28" s="2" t="s">
+      <c r="G28" s="15"/>
+      <c r="I28" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>52</v>
       </c>
@@ -2065,17 +2065,17 @@
       <c r="E29" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>53</v>
       </c>
@@ -2087,17 +2087,17 @@
       <c r="E30" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F30" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>54</v>
       </c>
@@ -2109,17 +2109,17 @@
       <c r="E31" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>55</v>
       </c>
@@ -2131,17 +2131,17 @@
       <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F32" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>59</v>
       </c>
@@ -2153,14 +2153,14 @@
       <c r="E33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>61</v>
       </c>
@@ -2172,14 +2172,14 @@
       <c r="E34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>63</v>
       </c>
@@ -2191,14 +2191,14 @@
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>68</v>
       </c>
@@ -2210,14 +2210,14 @@
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>69</v>
       </c>
@@ -2229,14 +2229,14 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>64</v>
       </c>
@@ -2248,14 +2248,14 @@
       <c r="E38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>67</v>
       </c>
@@ -2267,14 +2267,14 @@
       <c r="E39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>66</v>
       </c>
@@ -2286,14 +2286,14 @@
       <c r="E40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>65</v>
       </c>
@@ -2305,14 +2305,14 @@
       <c r="E41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>71</v>
       </c>
@@ -2324,14 +2324,14 @@
       <c r="E42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>73</v>
       </c>
@@ -2343,14 +2343,14 @@
       <c r="E43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>74</v>
       </c>
@@ -2362,14 +2362,14 @@
       <c r="E44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>72</v>
       </c>
@@ -2381,14 +2381,14 @@
       <c r="E45" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>80</v>
       </c>
@@ -2398,17 +2398,17 @@
       <c r="E46" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F46" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I46" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>81</v>
       </c>
@@ -2420,17 +2420,17 @@
       <c r="E47" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F47" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G47" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>87</v>
       </c>
@@ -2442,17 +2442,17 @@
       <c r="E48" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F48" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G48" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I48" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>88</v>
       </c>
@@ -2464,17 +2464,17 @@
       <c r="E49" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F49" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H49" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J49" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I49" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>89</v>
       </c>
@@ -2486,17 +2486,17 @@
       <c r="E50" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F50" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G50" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H50" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J50" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I50" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>85</v>
       </c>
@@ -2508,17 +2508,17 @@
       <c r="E51" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F51" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G51" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H51" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I51" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
@@ -2530,17 +2530,17 @@
       <c r="E52" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F52" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G52" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H52" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I52" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>90</v>
       </c>
@@ -2552,17 +2552,17 @@
       <c r="E53" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F53" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G53" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H53" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J53" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I53" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
@@ -2574,17 +2574,17 @@
       <c r="E54" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F54" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G54" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H54" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I54" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
@@ -2596,17 +2596,17 @@
       <c r="E55" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="F55" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H55" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J55" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I55" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -2618,14 +2618,14 @@
       <c r="E56" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="F56" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="J56" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I56" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -2637,14 +2637,14 @@
       <c r="E57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="F57" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="J57" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
@@ -2656,14 +2656,14 @@
       <c r="E58" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="F58" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="J58" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I58" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>99</v>
       </c>
@@ -2675,14 +2675,14 @@
       <c r="E59" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G59" s="15" t="s">
+      <c r="F59" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="J59" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I59" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>101</v>
       </c>
@@ -2694,14 +2694,14 @@
       <c r="E60" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G60" s="15" t="s">
+      <c r="F60" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="J60" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I60" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>103</v>
       </c>
@@ -2713,14 +2713,14 @@
       <c r="E61" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J61" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I61" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
@@ -2732,14 +2732,14 @@
       <c r="E62" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J62" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I62" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>105</v>
       </c>
@@ -2751,14 +2751,14 @@
       <c r="E63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J63" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I63" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>107</v>
       </c>
@@ -2770,14 +2770,14 @@
       <c r="E64" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="F64" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J64" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I64" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>110</v>
       </c>
@@ -2789,17 +2789,17 @@
       <c r="E65" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G65" s="15" t="s">
+      <c r="F65" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J65" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I65" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>111</v>
       </c>
@@ -2811,17 +2811,17 @@
       <c r="E66" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G66" s="15" t="s">
+      <c r="F66" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J66" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I66" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
         <v>114</v>
       </c>
@@ -2833,17 +2833,17 @@
       <c r="E67" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G67" s="15" t="s">
+      <c r="F67" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J67" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I67" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
@@ -2855,17 +2855,17 @@
       <c r="E68" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="F68" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J68" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I68" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>115</v>
       </c>
@@ -2877,17 +2877,17 @@
       <c r="E69" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G69" s="15" t="s">
+      <c r="F69" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J69" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I69" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="28.8" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>117</v>
       </c>
@@ -2899,17 +2899,17 @@
       <c r="E70" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G70" s="15" t="s">
+      <c r="F70" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J70" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I70" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>120</v>
       </c>
@@ -2921,17 +2921,17 @@
       <c r="E71" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G71" s="15" t="s">
+      <c r="F71" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J71" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I71" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>121</v>
       </c>
@@ -2943,17 +2943,17 @@
       <c r="E72" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G72" s="15" t="s">
+      <c r="F72" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J72" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I72" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>118</v>
       </c>
@@ -2965,17 +2965,17 @@
       <c r="E73" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G73" s="15" t="s">
+      <c r="F73" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J73" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I73" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>122</v>
       </c>
@@ -2987,17 +2987,17 @@
       <c r="E74" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="F74" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J74" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I74" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>123</v>
       </c>
@@ -3009,17 +3009,17 @@
       <c r="E75" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G75" s="15" t="s">
+      <c r="F75" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J75" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I75" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -3031,17 +3031,17 @@
       <c r="E76" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G76" s="15" t="s">
+      <c r="F76" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J76" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I76" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="28.8" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="s">
         <v>126</v>
       </c>
@@ -3053,17 +3053,17 @@
       <c r="E77" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G77" s="15" t="s">
+      <c r="F77" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J77" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I77" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>127</v>
       </c>
@@ -3075,17 +3075,17 @@
       <c r="E78" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G78" s="15" t="s">
+      <c r="F78" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J78" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I78" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>125</v>
       </c>
@@ -3097,17 +3097,17 @@
       <c r="E79" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G79" s="15" t="s">
+      <c r="F79" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J79" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I79" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>130</v>
       </c>
@@ -3119,26 +3119,26 @@
       <c r="E80" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>135</v>
       </c>
+      <c r="I80" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="J80" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K80" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="M80" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="N80" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P80" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>131</v>
       </c>
@@ -3150,23 +3150,23 @@
       <c r="E81" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J81" s="2" t="s">
-        <v>113</v>
+      <c r="I81" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P81" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>132</v>
       </c>
@@ -3178,23 +3178,23 @@
       <c r="E82" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J82" s="2" t="s">
-        <v>113</v>
+      <c r="I82" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P82" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>133</v>
       </c>
@@ -3206,23 +3206,23 @@
       <c r="E83" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J83" s="2" t="s">
-        <v>113</v>
+      <c r="I83" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P83" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>134</v>
       </c>
@@ -3234,23 +3234,23 @@
       <c r="E84" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J84" s="2" t="s">
-        <v>113</v>
+      <c r="I84" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P84" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>129</v>
       </c>
@@ -3262,23 +3262,23 @@
       <c r="E85" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J85" s="2" t="s">
-        <v>113</v>
+      <c r="I85" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="P85" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -3290,20 +3290,20 @@
       <c r="E86" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J86" s="2" t="s">
-        <v>113</v>
+      <c r="I86" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O86" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>140</v>
       </c>
@@ -3315,20 +3315,20 @@
       <c r="E87" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J87" s="2" t="s">
-        <v>113</v>
+      <c r="I87" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O87" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>141</v>
       </c>
@@ -3340,20 +3340,20 @@
       <c r="E88" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J88" s="2" t="s">
-        <v>113</v>
+      <c r="I88" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O88" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>142</v>
       </c>
@@ -3365,20 +3365,20 @@
       <c r="E89" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J89" s="2" t="s">
-        <v>113</v>
+      <c r="I89" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O89" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>143</v>
       </c>
@@ -3390,20 +3390,20 @@
       <c r="E90" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J90" s="2" t="s">
-        <v>113</v>
+      <c r="I90" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O90" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
         <v>149</v>
       </c>
@@ -3415,17 +3415,17 @@
       <c r="E91" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J91" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N91" s="26" t="s">
+      <c r="I91" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M91" s="26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>150</v>
       </c>
@@ -3437,20 +3437,20 @@
       <c r="E92" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J92" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N92" s="2" t="s">
+      <c r="I92" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M92" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q92" s="2" t="s">
+      <c r="P92" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>151</v>
       </c>
@@ -3462,20 +3462,20 @@
       <c r="E93" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J93" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N93" s="2" t="s">
+      <c r="I93" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M93" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q93" s="2" t="s">
+      <c r="P93" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>152</v>
       </c>
@@ -3487,17 +3487,17 @@
       <c r="E94" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="F94" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J94" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N94" s="2" t="s">
+      <c r="I94" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M94" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>153</v>
       </c>
@@ -3509,17 +3509,17 @@
       <c r="E95" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J95" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N95" s="2" t="s">
+      <c r="I95" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M95" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>154</v>
       </c>
@@ -3531,17 +3531,17 @@
       <c r="E96" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J96" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N96" s="2" t="s">
+      <c r="I96" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M96" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>155</v>
       </c>
@@ -3553,17 +3553,17 @@
       <c r="E97" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J97" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N97" s="2" t="s">
+      <c r="I97" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M97" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>148</v>
       </c>
@@ -3575,17 +3575,17 @@
       <c r="E98" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J98" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N98" s="2" t="s">
+      <c r="I98" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M98" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>158</v>
       </c>
@@ -3597,20 +3597,20 @@
       <c r="E99" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J99" s="2" t="s">
-        <v>113</v>
+      <c r="I99" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M99" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O99" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -3622,21 +3622,21 @@
       <c r="E100" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J100" s="2" t="s">
-        <v>113</v>
+      <c r="I100" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O100" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="R100" s="23"/>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q100" s="23"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>159</v>
       </c>
@@ -3648,20 +3648,20 @@
       <c r="E101" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J101" s="2" t="s">
-        <v>113</v>
+      <c r="I101" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O101" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>162</v>
       </c>
@@ -3673,14 +3673,14 @@
       <c r="E102" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J102" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I102" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>163</v>
       </c>
@@ -3692,14 +3692,14 @@
       <c r="E103" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J103" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I103" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>166</v>
       </c>
@@ -3711,17 +3711,17 @@
       <c r="E104" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="F104" s="1" t="s">
         <v>165</v>
       </c>
+      <c r="I104" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="J104" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K104" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>169</v>
       </c>
@@ -3733,14 +3733,14 @@
       <c r="E105" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G105" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J105" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I105" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>168</v>
       </c>
@@ -3752,14 +3752,14 @@
       <c r="E106" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G106" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J106" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I106" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>167</v>
       </c>
@@ -3771,14 +3771,14 @@
       <c r="E107" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J107" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I107" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>171</v>
       </c>
@@ -3790,23 +3790,23 @@
       <c r="E108" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="F108" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J108" s="2" t="s">
-        <v>113</v>
+      <c r="I108" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M108" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O108" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q108" s="2" t="s">
+      <c r="P108" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>174</v>
       </c>
@@ -3818,23 +3818,23 @@
       <c r="E109" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J109" s="2" t="s">
-        <v>113</v>
+      <c r="I109" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M109" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O109" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q109" s="2" t="s">
+      <c r="P109" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>175</v>
       </c>
@@ -3846,23 +3846,23 @@
       <c r="E110" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J110" s="2" t="s">
-        <v>113</v>
+      <c r="I110" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M110" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O110" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q110" s="2" t="s">
+      <c r="P110" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>172</v>
       </c>
@@ -3874,23 +3874,23 @@
       <c r="E111" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J111" s="2" t="s">
-        <v>113</v>
+      <c r="I111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M111" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O111" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q111" s="2" t="s">
+      <c r="P111" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>176</v>
       </c>
@@ -3902,23 +3902,23 @@
       <c r="E112" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J112" s="2" t="s">
-        <v>113</v>
+      <c r="I112" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M112" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O112" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q112" s="2" t="s">
+      <c r="P112" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>177</v>
       </c>
@@ -3930,23 +3930,23 @@
       <c r="E113" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="F113" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J113" s="2" t="s">
-        <v>113</v>
+      <c r="I113" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M113" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O113" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q113" s="2" t="s">
+      <c r="P113" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>178</v>
       </c>
@@ -3958,23 +3958,23 @@
       <c r="E114" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="F114" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J114" s="2" t="s">
-        <v>113</v>
+      <c r="I114" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M114" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O114" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q114" s="2" t="s">
+      <c r="P114" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>173</v>
       </c>
@@ -3986,23 +3986,23 @@
       <c r="E115" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J115" s="2" t="s">
-        <v>113</v>
+      <c r="I115" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="O115" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="Q115" s="2" t="s">
+      <c r="P115" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>182</v>
       </c>
@@ -4014,14 +4014,14 @@
       <c r="E116" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J116" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I116" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>183</v>
       </c>
@@ -4033,14 +4033,14 @@
       <c r="E117" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J117" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I117" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>186</v>
       </c>
@@ -4052,14 +4052,14 @@
       <c r="E118" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G118" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="J118" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="119" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I118" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>185</v>
       </c>
@@ -4071,23 +4071,23 @@
       <c r="E119" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G119" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="J119" s="2" t="s">
-        <v>113</v>
+      <c r="I119" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="N119" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="P119" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="O119" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q119" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>190</v>
       </c>
@@ -4099,14 +4099,14 @@
       <c r="E120" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G120" s="25" t="s">
+      <c r="F120" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="J120" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I120" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>191</v>
       </c>
@@ -4118,11 +4118,11 @@
       <c r="E121" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J121" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I121" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
         <v>192</v>
       </c>
@@ -4134,11 +4134,11 @@
       <c r="E122" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J122" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I122" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>196</v>
       </c>
@@ -4150,14 +4150,14 @@
       <c r="E123" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G123" s="27" t="s">
+      <c r="F123" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="J123" s="2" t="s">
+      <c r="I123" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>198</v>
       </c>
@@ -4169,14 +4169,14 @@
       <c r="E124" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G124" s="27" t="s">
+      <c r="F124" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="J124" s="2" t="s">
+      <c r="I124" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>199</v>
       </c>
@@ -4188,14 +4188,14 @@
       <c r="E125" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G125" s="27" t="s">
+      <c r="F125" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="I125" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>200</v>
       </c>
@@ -4207,14 +4207,14 @@
       <c r="E126" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G126" s="27" t="s">
+      <c r="F126" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="J126" s="2" t="s">
+      <c r="I126" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>197</v>
       </c>
@@ -4226,14 +4226,14 @@
       <c r="E127" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G127" s="27" t="s">
+      <c r="F127" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="J127" s="2" t="s">
+      <c r="I127" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="s">
         <v>201</v>
       </c>
@@ -4245,14 +4245,14 @@
       <c r="E128" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G128" s="25" t="s">
+      <c r="F128" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="J128" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I128" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>202</v>
       </c>
@@ -4264,14 +4264,14 @@
       <c r="E129" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G129" s="25" t="s">
+      <c r="F129" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="J129" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I129" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>206</v>
       </c>
@@ -4283,14 +4283,14 @@
       <c r="E130" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="F130" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="J130" s="2" t="s">
+      <c r="I130" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>207</v>
       </c>
@@ -4302,14 +4302,14 @@
       <c r="E131" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="F131" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="J131" s="2" t="s">
+      <c r="I131" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>210</v>
       </c>
@@ -4321,14 +4321,14 @@
       <c r="E132" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="F132" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J132" s="2" t="s">
+      <c r="I132" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>211</v>
       </c>
@@ -4340,14 +4340,14 @@
       <c r="E133" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="F133" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J133" s="2" t="s">
+      <c r="I133" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>209</v>
       </c>
@@ -4359,14 +4359,14 @@
       <c r="E134" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J134" s="2" t="s">
+      <c r="I134" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>213</v>
       </c>
@@ -4378,11 +4378,11 @@
       <c r="E135" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J135" s="2" t="s">
+      <c r="I135" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>215</v>
       </c>
@@ -4394,11 +4394,11 @@
       <c r="E136" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J136" s="2" t="s">
+      <c r="I136" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>214</v>
       </c>
@@ -4410,11 +4410,11 @@
       <c r="E137" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J137" s="2" t="s">
+      <c r="I137" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>217</v>
       </c>
@@ -4426,17 +4426,17 @@
       <c r="E138" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G138" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="I138" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="J138" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K138" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>218</v>
       </c>
@@ -4448,17 +4448,17 @@
       <c r="E139" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G139" s="1" t="s">
+      <c r="F139" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="I139" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="J139" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K139" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>219</v>
       </c>
@@ -4470,17 +4470,17 @@
       <c r="E140" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G140" s="1" t="s">
+      <c r="F140" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="I140" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="J140" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K140" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>220</v>
       </c>
@@ -4492,17 +4492,17 @@
       <c r="E141" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G141" s="1" t="s">
+      <c r="F141" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="I141" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="J141" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K141" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4510,95 +4510,95 @@
         <v>238</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
-      <c r="H156" s="2" t="s">
+      <c r="G156" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -4615,8 +4615,8 @@
     <row r="170" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="171" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:T142" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="6">
+  <autoFilter ref="A1:S142" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="5">
       <filters blank="1">
         <filter val="5-NITRO-IMIDAZOLES "/>
         <filter val="ANALOGUES NUCLEOSIDIQUES"/>

</xml_diff>